<commit_message>
Supervisors; maximum number of students per supervisor (easy); maximum number of projects per supervisor (harder). Hat-tip to Stevens & Palocsay (2017).
</commit_message>
<xml_diff>
--- a/pdn_project_allocation/testdata/test1_equal_preferences_check_output_consistency.xlsx
+++ b/pdn_project_allocation/testdata/test1_equal_preferences_check_output_consistency.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Projects" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Student_preferences" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Supervisor_preferences" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Supervisors" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Projects" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Student_preferences" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Supervisor_preferences" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,12 +23,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">Project_name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
+  <si>
+    <t xml:space="preserve">Supervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max_number_of_projects</t>
   </si>
   <si>
     <t xml:space="preserve">Max_number_of_students</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dr Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project</t>
   </si>
   <si>
     <t xml:space="preserve">Morris water maze</t>
@@ -146,79 +156,140 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.91"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="B6:F6 B7"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -232,18 +303,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6:F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.55"/>
@@ -251,32 +322,31 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -296,7 +366,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1</v>
@@ -316,7 +386,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -336,7 +406,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1</v>
@@ -356,7 +426,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -385,62 +455,59 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B6:F6 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>